<commit_message>
Updates to test and move to tox.
</commit_message>
<xml_diff>
--- a/tests/data/expected-integers.xlsx
+++ b/tests/data/expected-integers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="IntegerModel" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="step_1" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="step_2" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="step_3" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="IntegerModel" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="step_1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="step_2" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="step_3" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -47,15 +47,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -356,7 +356,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="2.14" customWidth="1" min="1" max="1"/>
+    <col customWidth="1" max="1" min="1" width="2.14"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -491,7 +491,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -509,8 +509,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="2.14" customWidth="1" min="1" max="1"/>
-    <col width="12" customWidth="1" min="2" max="2"/>
+    <col customWidth="1" max="1" min="1" width="2.14"/>
+    <col customWidth="1" max="2" min="2" width="12"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -632,7 +632,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -650,8 +650,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="2.14" customWidth="1" min="1" max="1"/>
-    <col width="12" customWidth="1" min="2" max="2"/>
+    <col customWidth="1" max="1" min="1" width="2.14"/>
+    <col customWidth="1" max="2" min="2" width="12"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -773,7 +773,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -791,8 +791,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="2.14" customWidth="1" min="1" max="1"/>
-    <col width="12" customWidth="1" min="2" max="2"/>
+    <col customWidth="1" max="1" min="1" width="2.14"/>
+    <col customWidth="1" max="2" min="2" width="12"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -928,6 +928,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Renamed Placeholder to Intermediate, Asset to Return, and Modifier to Sensitivity.
</commit_message>
<xml_diff>
--- a/tests/data/expected-integers.xlsx
+++ b/tests/data/expected-integers.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:C34"/>
+  <dimension ref="B2:C37"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>IntegerModel(*, a: 'int', b: 'int', c: 'int', d: 'int') -&gt; 'IntegerModel'</t>
+          <t>IntegerModel(*, a: int, b: int, c: int, d: int) -&gt; 'IntegerModel'</t>
         </is>
       </c>
     </row>
@@ -553,14 +553,14 @@
     <row r="19">
       <c r="C19" t="inlineStr">
         <is>
-          <t>Assets</t>
+          <t>Intermediates</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="C20" t="inlineStr">
         <is>
-          <t>------</t>
+          <t>-------------</t>
         </is>
       </c>
     </row>
@@ -593,59 +593,76 @@
       </c>
     </row>
     <row r="25">
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>ret_3 : int</t>
-        </is>
-      </c>
+      <c r="C25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="C26" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Result total of step_1 and step_2</t>
+          <t>Returns</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="C27" t="inlineStr"/>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>-------</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="C28" t="inlineStr">
         <is>
-          <t>Steps</t>
+          <t>ret_3 : int</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="C29" t="inlineStr">
         <is>
-          <t>-----</t>
+          <t xml:space="preserve">    Result total of step_1 and step_2</t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>1. _step_1 - Add a and b together.</t>
-        </is>
-      </c>
+      <c r="C30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="C31" t="inlineStr">
         <is>
-          <t>2. _step_2 - Subtract d from c</t>
+          <t>Steps</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="C32" t="inlineStr">
         <is>
-          <t>3. _step_3 - Add total of steps 1 and 2.</t>
+          <t>-----</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>1) _step_1 - Add a and b together.</t>
         </is>
       </c>
     </row>
     <row r="34">
-      <c r="C34" t="inlineStr"/>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>2) _step_2 - Subtract d from c</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>3) _step_3 - Add total of steps 1 and 2.</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="C37" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -804,7 +821,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>[asset.ret_1]</t>
+          <t>[intermediate.ret_1]</t>
         </is>
       </c>
     </row>
@@ -830,7 +847,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>asset.ret_1</t>
+          <t>intermediate.ret_1</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -923,7 +940,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>[asset.ret_2]</t>
+          <t>[intermediate.ret_2]</t>
         </is>
       </c>
     </row>
@@ -949,7 +966,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>asset.ret_2</t>
+          <t>intermediate.ret_2</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -977,7 +994,7 @@
   <cols>
     <col width="2.14" customWidth="1" min="1" max="1"/>
     <col width="14" customWidth="1" min="2" max="2"/>
-    <col width="30" customWidth="1" min="3" max="3"/>
+    <col width="43" customWidth="1" min="3" max="3"/>
     <col width="7" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
@@ -1029,7 +1046,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>[asset.ret_1, asset.ret_2]</t>
+          <t>[intermediate.ret_1, intermediate.ret_2]</t>
         </is>
       </c>
     </row>
@@ -1042,7 +1059,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>[asset.ret_3]</t>
+          <t>[return.ret_3]</t>
         </is>
       </c>
     </row>
@@ -1068,7 +1085,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>asset.ret_3</t>
+          <t>return.ret_3</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -1086,7 +1103,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1109,30 +1126,10 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ret_1</t>
+          <t>ret_3</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>ret_2</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>ret_3</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1147,7 +1144,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K95"/>
+  <dimension ref="A1:K94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2157,13 +2154,13 @@
         </is>
       </c>
       <c r="H34" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I34" t="n">
         <v>3</v>
       </c>
       <c r="J34" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K34" t="n">
         <v>3</v>
@@ -2172,12 +2169,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Instantiation</t>
+          <t>Main</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>INSTANTIATION</t>
+          <t>DOCSTRING</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -2186,37 +2183,27 @@
         </is>
       </c>
       <c r="H35" t="n">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="I35" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J35" t="n">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="K35" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Instantiation</t>
+          <t>Main</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>INSTANTIATION</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>[parameter.a]</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>KEY</t>
+          <t>DOCSTRING</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -2225,13 +2212,13 @@
         </is>
       </c>
       <c r="H36" t="n">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="I36" t="n">
         <v>3</v>
       </c>
       <c r="J36" t="n">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="K36" t="n">
         <v>3</v>
@@ -2240,40 +2227,30 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Instantiation</t>
+          <t>Main</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>INSTANTIATION</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>[parameter.a]</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>VALUE</t>
+          <t>DOCSTRING</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>&lt;class 'int'&gt;</t>
+          <t>&lt;class 'str'&gt;</t>
         </is>
       </c>
       <c r="H37" t="n">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="I37" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J37" t="n">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="K37" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38">
@@ -2287,32 +2264,22 @@
           <t>INSTANTIATION</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>[parameter.b]</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>KEY</t>
-        </is>
-      </c>
       <c r="F38" t="inlineStr">
         <is>
           <t>&lt;class 'str'&gt;</t>
         </is>
       </c>
       <c r="H38" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I38" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J38" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K38" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39">
@@ -2328,30 +2295,30 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>[parameter.b]</t>
+          <t>[parameter.a]</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>VALUE</t>
+          <t>KEY</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>&lt;class 'int'&gt;</t>
+          <t>&lt;class 'str'&gt;</t>
         </is>
       </c>
       <c r="H39" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I39" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J39" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K39" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40">
@@ -2367,30 +2334,30 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>[parameter.c]</t>
+          <t>[parameter.a]</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>KEY</t>
+          <t>VALUE</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>&lt;class 'str'&gt;</t>
+          <t>&lt;class 'int'&gt;</t>
         </is>
       </c>
       <c r="H40" t="n">
+        <v>2</v>
+      </c>
+      <c r="I40" t="n">
         <v>4</v>
       </c>
-      <c r="I40" t="n">
-        <v>3</v>
-      </c>
       <c r="J40" t="n">
+        <v>2</v>
+      </c>
+      <c r="K40" t="n">
         <v>4</v>
-      </c>
-      <c r="K40" t="n">
-        <v>3</v>
       </c>
     </row>
     <row r="41">
@@ -2406,30 +2373,30 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>[parameter.c]</t>
+          <t>[parameter.b]</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>VALUE</t>
+          <t>KEY</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>&lt;class 'int'&gt;</t>
+          <t>&lt;class 'str'&gt;</t>
         </is>
       </c>
       <c r="H41" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I41" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J41" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K41" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42">
@@ -2445,30 +2412,30 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>[parameter.d]</t>
+          <t>[parameter.b]</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>KEY</t>
+          <t>VALUE</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>&lt;class 'str'&gt;</t>
+          <t>&lt;class 'int'&gt;</t>
         </is>
       </c>
       <c r="H42" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I42" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J42" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K42" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43">
@@ -2484,70 +2451,90 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>[parameter.d]</t>
+          <t>[parameter.c]</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>VALUE</t>
+          <t>KEY</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>&lt;class 'int'&gt;</t>
+          <t>&lt;class 'str'&gt;</t>
         </is>
       </c>
       <c r="H43" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I43" t="n">
+        <v>3</v>
+      </c>
+      <c r="J43" t="n">
         <v>4</v>
       </c>
-      <c r="J43" t="n">
-        <v>5</v>
-      </c>
       <c r="K43" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>_step_1</t>
+          <t>Instantiation</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>NAME</t>
+          <t>INSTANTIATION</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>[parameter.c]</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>VALUE</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>&lt;class 'str'&gt;</t>
+          <t>&lt;class 'int'&gt;</t>
         </is>
       </c>
       <c r="H44" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I44" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J44" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K44" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>_step_1</t>
+          <t>Instantiation</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>NAME</t>
+          <t>INSTANTIATION</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>[parameter.d]</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>KEY</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -2556,13 +2543,13 @@
         </is>
       </c>
       <c r="H45" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I45" t="n">
         <v>3</v>
       </c>
       <c r="J45" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K45" t="n">
         <v>3</v>
@@ -2571,30 +2558,40 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>_step_1</t>
+          <t>Instantiation</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>MTEHOD_NAME</t>
+          <t>INSTANTIATION</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>[parameter.d]</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>VALUE</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>&lt;class 'str'&gt;</t>
+          <t>&lt;class 'int'&gt;</t>
         </is>
       </c>
       <c r="H46" t="n">
+        <v>5</v>
+      </c>
+      <c r="I46" t="n">
         <v>4</v>
       </c>
-      <c r="I46" t="n">
-        <v>2</v>
-      </c>
       <c r="J46" t="n">
+        <v>5</v>
+      </c>
+      <c r="K46" t="n">
         <v>4</v>
-      </c>
-      <c r="K46" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="47">
@@ -2605,7 +2602,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>MTEHOD_NAME</t>
+          <t>NAME</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -2614,16 +2611,16 @@
         </is>
       </c>
       <c r="H47" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I47" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J47" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K47" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48">
@@ -2634,7 +2631,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>DOCSTRING</t>
+          <t>NAME</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -2643,16 +2640,16 @@
         </is>
       </c>
       <c r="H48" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I48" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J48" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K48" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49">
@@ -2663,7 +2660,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>DOCSTRING</t>
+          <t>MTEHOD_NAME</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -2672,16 +2669,16 @@
         </is>
       </c>
       <c r="H49" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I49" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J49" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K49" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50">
@@ -2692,7 +2689,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>USES</t>
+          <t>MTEHOD_NAME</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -2701,16 +2698,16 @@
         </is>
       </c>
       <c r="H50" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I50" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J50" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K50" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51">
@@ -2721,7 +2718,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>USES</t>
+          <t>DOCSTRING</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -2730,16 +2727,16 @@
         </is>
       </c>
       <c r="H51" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I51" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J51" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K51" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52">
@@ -2750,7 +2747,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>IMPACTS</t>
+          <t>DOCSTRING</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -2759,16 +2756,16 @@
         </is>
       </c>
       <c r="H52" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="I52" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J52" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="K52" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="53">
@@ -2779,7 +2776,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>IMPACTS</t>
+          <t>USES</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -2788,16 +2785,16 @@
         </is>
       </c>
       <c r="H53" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I53" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J53" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="K53" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54">
@@ -2808,7 +2805,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>METADATA</t>
+          <t>USES</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -2817,16 +2814,16 @@
         </is>
       </c>
       <c r="H54" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I54" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J54" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K54" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="55">
@@ -2837,7 +2834,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>METADATA</t>
+          <t>IMPACTS</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -2846,16 +2843,16 @@
         </is>
       </c>
       <c r="H55" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I55" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J55" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="K55" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56">
@@ -2866,7 +2863,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>OUTPUT</t>
+          <t>IMPACTS</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -2875,16 +2872,16 @@
         </is>
       </c>
       <c r="H56" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="I56" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J56" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="K56" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57">
@@ -2895,17 +2892,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>OUTPUT</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>[asset.ret_1]</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>KEY</t>
+          <t>METADATA</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -2914,16 +2901,16 @@
         </is>
       </c>
       <c r="H57" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I57" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J57" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K57" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58">
@@ -2934,46 +2921,36 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>OUTPUT</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>[asset.ret_1]</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>VALUE</t>
+          <t>METADATA</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>&lt;class 'int'&gt;</t>
+          <t>&lt;class 'str'&gt;</t>
         </is>
       </c>
       <c r="H58" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I58" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J58" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K58" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>_step_2</t>
+          <t>_step_1</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>NAME</t>
+          <t>OUTPUT</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -2982,13 +2959,13 @@
         </is>
       </c>
       <c r="H59" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="I59" t="n">
         <v>2</v>
       </c>
       <c r="J59" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="K59" t="n">
         <v>2</v>
@@ -2997,12 +2974,22 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>_step_2</t>
+          <t>_step_1</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>NAME</t>
+          <t>OUTPUT</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>[intermediate.ret_1]</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>KEY</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -3011,13 +2998,13 @@
         </is>
       </c>
       <c r="H60" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="I60" t="n">
         <v>3</v>
       </c>
       <c r="J60" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="K60" t="n">
         <v>3</v>
@@ -3026,30 +3013,40 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>_step_2</t>
+          <t>_step_1</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>MTEHOD_NAME</t>
+          <t>OUTPUT</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>[intermediate.ret_1]</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>VALUE</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>&lt;class 'str'&gt;</t>
+          <t>&lt;class 'int'&gt;</t>
         </is>
       </c>
       <c r="H61" t="n">
+        <v>14</v>
+      </c>
+      <c r="I61" t="n">
         <v>4</v>
       </c>
-      <c r="I61" t="n">
-        <v>2</v>
-      </c>
       <c r="J61" t="n">
+        <v>14</v>
+      </c>
+      <c r="K61" t="n">
         <v>4</v>
-      </c>
-      <c r="K61" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="62">
@@ -3060,7 +3057,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>MTEHOD_NAME</t>
+          <t>NAME</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -3069,16 +3066,16 @@
         </is>
       </c>
       <c r="H62" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I62" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J62" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K62" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63">
@@ -3089,7 +3086,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>DOCSTRING</t>
+          <t>NAME</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -3098,16 +3095,16 @@
         </is>
       </c>
       <c r="H63" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I63" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J63" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K63" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64">
@@ -3118,7 +3115,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>DOCSTRING</t>
+          <t>MTEHOD_NAME</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -3127,16 +3124,16 @@
         </is>
       </c>
       <c r="H64" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I64" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J64" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K64" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="65">
@@ -3147,7 +3144,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>USES</t>
+          <t>MTEHOD_NAME</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -3156,16 +3153,16 @@
         </is>
       </c>
       <c r="H65" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I65" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J65" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K65" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="66">
@@ -3176,7 +3173,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>USES</t>
+          <t>DOCSTRING</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -3185,16 +3182,16 @@
         </is>
       </c>
       <c r="H66" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I66" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J66" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K66" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="67">
@@ -3205,7 +3202,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>IMPACTS</t>
+          <t>DOCSTRING</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -3214,16 +3211,16 @@
         </is>
       </c>
       <c r="H67" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="I67" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J67" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="K67" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="68">
@@ -3234,7 +3231,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>IMPACTS</t>
+          <t>USES</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -3243,16 +3240,16 @@
         </is>
       </c>
       <c r="H68" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I68" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J68" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="K68" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69">
@@ -3263,7 +3260,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>METADATA</t>
+          <t>USES</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -3272,16 +3269,16 @@
         </is>
       </c>
       <c r="H69" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I69" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J69" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K69" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="70">
@@ -3292,7 +3289,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>METADATA</t>
+          <t>IMPACTS</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -3301,16 +3298,16 @@
         </is>
       </c>
       <c r="H70" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I70" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J70" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="K70" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71">
@@ -3321,7 +3318,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>OUTPUT</t>
+          <t>IMPACTS</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -3330,16 +3327,16 @@
         </is>
       </c>
       <c r="H71" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="I71" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J71" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="K71" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="72">
@@ -3350,17 +3347,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>OUTPUT</t>
-        </is>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>[asset.ret_2]</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>KEY</t>
+          <t>METADATA</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -3369,16 +3356,16 @@
         </is>
       </c>
       <c r="H72" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I72" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J72" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K72" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="73">
@@ -3389,46 +3376,36 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>OUTPUT</t>
-        </is>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>[asset.ret_2]</t>
-        </is>
-      </c>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>VALUE</t>
+          <t>METADATA</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>&lt;class 'int'&gt;</t>
+          <t>&lt;class 'str'&gt;</t>
         </is>
       </c>
       <c r="H73" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I73" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J73" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K73" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>_step_3</t>
+          <t>_step_2</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>NAME</t>
+          <t>OUTPUT</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -3437,13 +3414,13 @@
         </is>
       </c>
       <c r="H74" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="I74" t="n">
         <v>2</v>
       </c>
       <c r="J74" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="K74" t="n">
         <v>2</v>
@@ -3452,12 +3429,22 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>_step_3</t>
+          <t>_step_2</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>NAME</t>
+          <t>OUTPUT</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>[intermediate.ret_2]</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>KEY</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -3466,13 +3453,13 @@
         </is>
       </c>
       <c r="H75" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="I75" t="n">
         <v>3</v>
       </c>
       <c r="J75" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="K75" t="n">
         <v>3</v>
@@ -3481,30 +3468,40 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>_step_3</t>
+          <t>_step_2</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>MTEHOD_NAME</t>
+          <t>OUTPUT</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>[intermediate.ret_2]</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>VALUE</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>&lt;class 'str'&gt;</t>
+          <t>&lt;class 'int'&gt;</t>
         </is>
       </c>
       <c r="H76" t="n">
+        <v>14</v>
+      </c>
+      <c r="I76" t="n">
         <v>4</v>
       </c>
-      <c r="I76" t="n">
-        <v>2</v>
-      </c>
       <c r="J76" t="n">
+        <v>14</v>
+      </c>
+      <c r="K76" t="n">
         <v>4</v>
-      </c>
-      <c r="K76" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="77">
@@ -3515,7 +3512,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>MTEHOD_NAME</t>
+          <t>NAME</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -3524,16 +3521,16 @@
         </is>
       </c>
       <c r="H77" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I77" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J77" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K77" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="78">
@@ -3544,7 +3541,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>DOCSTRING</t>
+          <t>NAME</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -3553,16 +3550,16 @@
         </is>
       </c>
       <c r="H78" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I78" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J78" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K78" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="79">
@@ -3573,7 +3570,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>DOCSTRING</t>
+          <t>MTEHOD_NAME</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -3582,16 +3579,16 @@
         </is>
       </c>
       <c r="H79" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I79" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J79" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K79" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="80">
@@ -3602,7 +3599,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>USES</t>
+          <t>MTEHOD_NAME</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -3611,16 +3608,16 @@
         </is>
       </c>
       <c r="H80" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I80" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J80" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K80" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="81">
@@ -3631,7 +3628,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>USES</t>
+          <t>DOCSTRING</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -3640,16 +3637,16 @@
         </is>
       </c>
       <c r="H81" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I81" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J81" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K81" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="82">
@@ -3660,7 +3657,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>IMPACTS</t>
+          <t>DOCSTRING</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -3669,16 +3666,16 @@
         </is>
       </c>
       <c r="H82" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="I82" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J82" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="K82" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="83">
@@ -3689,7 +3686,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>IMPACTS</t>
+          <t>USES</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -3698,16 +3695,16 @@
         </is>
       </c>
       <c r="H83" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I83" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J83" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="K83" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="84">
@@ -3718,7 +3715,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>METADATA</t>
+          <t>USES</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -3727,16 +3724,16 @@
         </is>
       </c>
       <c r="H84" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I84" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J84" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K84" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="85">
@@ -3747,7 +3744,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>METADATA</t>
+          <t>IMPACTS</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -3756,16 +3753,16 @@
         </is>
       </c>
       <c r="H85" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I85" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J85" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="K85" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="86">
@@ -3776,7 +3773,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>OUTPUT</t>
+          <t>IMPACTS</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -3785,16 +3782,16 @@
         </is>
       </c>
       <c r="H86" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="I86" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J86" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="K86" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="87">
@@ -3805,17 +3802,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>OUTPUT</t>
-        </is>
-      </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>[asset.ret_3]</t>
-        </is>
-      </c>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>KEY</t>
+          <t>METADATA</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -3824,16 +3811,16 @@
         </is>
       </c>
       <c r="H87" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I87" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J87" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K87" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="88">
@@ -3844,41 +3831,31 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>OUTPUT</t>
-        </is>
-      </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>[asset.ret_3]</t>
-        </is>
-      </c>
-      <c r="D88" t="inlineStr">
-        <is>
-          <t>VALUE</t>
+          <t>METADATA</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>&lt;class 'int'&gt;</t>
+          <t>&lt;class 'str'&gt;</t>
         </is>
       </c>
       <c r="H88" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I88" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J88" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K88" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Output</t>
+          <t>_step_3</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -3892,13 +3869,13 @@
         </is>
       </c>
       <c r="H89" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="I89" t="n">
         <v>2</v>
       </c>
       <c r="J89" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="K89" t="n">
         <v>2</v>
@@ -3907,7 +3884,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Output</t>
+          <t>_step_3</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -3917,7 +3894,7 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>[ret_1]</t>
+          <t>[return.ret_3]</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -3931,13 +3908,13 @@
         </is>
       </c>
       <c r="H90" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="I90" t="n">
         <v>3</v>
       </c>
       <c r="J90" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="K90" t="n">
         <v>3</v>
@@ -3946,7 +3923,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Output</t>
+          <t>_step_3</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -3956,7 +3933,7 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>[ret_1]</t>
+          <t>[return.ret_3]</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
@@ -3970,13 +3947,13 @@
         </is>
       </c>
       <c r="H91" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="I91" t="n">
         <v>4</v>
       </c>
       <c r="J91" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="K91" t="n">
         <v>4</v>
@@ -3993,32 +3970,22 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>[ret_2]</t>
-        </is>
-      </c>
-      <c r="D92" t="inlineStr">
-        <is>
-          <t>KEY</t>
-        </is>
-      </c>
       <c r="F92" t="inlineStr">
         <is>
           <t>&lt;class 'str'&gt;</t>
         </is>
       </c>
       <c r="H92" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I92" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J92" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K92" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="93">
@@ -4034,30 +4001,30 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>[ret_2]</t>
+          <t>[ret_3]</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>VALUE</t>
+          <t>KEY</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>&lt;class 'int'&gt;</t>
+          <t>&lt;class 'str'&gt;</t>
         </is>
       </c>
       <c r="H93" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I93" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J93" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K93" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="94">
@@ -4078,63 +4045,24 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>KEY</t>
+          <t>VALUE</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>&lt;class 'str'&gt;</t>
+          <t>&lt;class 'int'&gt;</t>
         </is>
       </c>
       <c r="H94" t="n">
+        <v>2</v>
+      </c>
+      <c r="I94" t="n">
         <v>4</v>
       </c>
-      <c r="I94" t="n">
-        <v>3</v>
-      </c>
       <c r="J94" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K94" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>Output</t>
-        </is>
-      </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>OUTPUT</t>
-        </is>
-      </c>
-      <c r="C95" t="inlineStr">
-        <is>
-          <t>[ret_3]</t>
-        </is>
-      </c>
-      <c r="D95" t="inlineStr">
-        <is>
-          <t>VALUE</t>
-        </is>
-      </c>
-      <c r="F95" t="inlineStr">
-        <is>
-          <t>&lt;class 'int'&gt;</t>
-        </is>
-      </c>
-      <c r="H95" t="n">
-        <v>4</v>
-      </c>
-      <c r="I95" t="n">
-        <v>4</v>
-      </c>
-      <c r="J95" t="n">
-        <v>4</v>
-      </c>
-      <c r="K95" t="n">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactored audit to return AuditContainer vs dict.
</commit_message>
<xml_diff>
--- a/tests/data/expected-integers.xlsx
+++ b/tests/data/expected-integers.xlsx
@@ -808,7 +808,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>[parameter.a, parameter.b]</t>
+          <t>(parameter.a, parameter.b)</t>
         </is>
       </c>
     </row>
@@ -821,7 +821,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>[intermediate.ret_1]</t>
+          <t>(intermediate.ret_1,)</t>
         </is>
       </c>
     </row>
@@ -927,7 +927,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>[parameter.c, parameter.d]</t>
+          <t>(parameter.c, parameter.d)</t>
         </is>
       </c>
     </row>
@@ -940,7 +940,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>[intermediate.ret_2]</t>
+          <t>(intermediate.ret_2,)</t>
         </is>
       </c>
     </row>
@@ -1046,7 +1046,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>[intermediate.ret_1, intermediate.ret_2]</t>
+          <t>(intermediate.ret_1, intermediate.ret_2)</t>
         </is>
       </c>
     </row>
@@ -1059,7 +1059,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>[return.ret_3]</t>
+          <t>(return.ret_3,)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated how the docstring is generated for models and fixed any associated test.
</commit_message>
<xml_diff>
--- a/tests/data/expected-integers.xlsx
+++ b/tests/data/expected-integers.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:C37"/>
+  <dimension ref="B2:C31"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,115 +483,95 @@
     <row r="8">
       <c r="C8" t="inlineStr">
         <is>
-          <t>Parameters</t>
+          <t>.. rubric:: Parameters</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>----------</t>
-        </is>
-      </c>
+      <c r="C9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="C10" t="inlineStr">
         <is>
-          <t>a : int</t>
+          <t>- **a (int)** - A number A</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="C11" t="inlineStr">
         <is>
-          <t xml:space="preserve">    A number A</t>
+          <t>- **b (int)** - A number B</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="C12" t="inlineStr">
         <is>
-          <t>b : int</t>
+          <t>- **c (int)** - A number C</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="C13" t="inlineStr">
         <is>
-          <t xml:space="preserve">    A number B</t>
+          <t>- **d (int)** - A number D</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>c : int</t>
-        </is>
-      </c>
+      <c r="C14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="C15" t="inlineStr">
         <is>
-          <t xml:space="preserve">    A number C</t>
+          <t>.. rubric:: Intermediates</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>d : int</t>
-        </is>
-      </c>
+      <c r="C16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="C17" t="inlineStr">
         <is>
-          <t xml:space="preserve">    A number D</t>
+          <t>- **ret_1 (int)** - Results a + b</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="C18" t="inlineStr"/>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>- **ret_2 (int)** - Results c - d</t>
+        </is>
+      </c>
     </row>
     <row r="19">
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Intermediates</t>
-        </is>
-      </c>
+      <c r="C19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="C20" t="inlineStr">
         <is>
-          <t>-------------</t>
+          <t>.. rubric:: Returns</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>ret_1 : int</t>
-        </is>
-      </c>
+      <c r="C21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="C22" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Results a + b</t>
+          <t>- **ret_3 (int)** - Result total of step_1 and step_2</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>ret_2 : int</t>
-        </is>
-      </c>
+      <c r="C23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="C24" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Results c - d</t>
+          <t>.. rubric:: Steps</t>
         </is>
       </c>
     </row>
@@ -601,71 +581,29 @@
     <row r="26">
       <c r="C26" t="inlineStr">
         <is>
-          <t>Returns</t>
+          <t>1) **_step_1** - Add a and b together.</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="C27" t="inlineStr">
         <is>
-          <t>-------</t>
+          <t>2) **_step_2** - Subtract d from c</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="C28" t="inlineStr">
         <is>
-          <t>ret_3 : int</t>
+          <t>3) **_step_3** - Add total of steps 1 and 2.</t>
         </is>
       </c>
     </row>
     <row r="29">
-      <c r="C29" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    Result total of step_1 and step_2</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="C30" t="inlineStr"/>
+      <c r="C29" t="inlineStr"/>
     </row>
     <row r="31">
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>Steps</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>-----</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>1) _step_1 - Add a and b together.</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>2) _step_2 - Subtract d from c</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>3) _step_3 - Add total of steps 1 and 2.</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="C37" t="inlineStr"/>
+      <c r="C31" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1291,7 +1229,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G114"/>
+  <dimension ref="A1:G108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2194,13 +2132,13 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E31" t="n">
         <v>3</v>
       </c>
       <c r="F31" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G31" t="n">
         <v>3</v>
@@ -2209,12 +2147,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Main</t>
+          <t>Instantiation</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>/docstring</t>
+          <t>/instantiation</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -2223,27 +2161,27 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="E32" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F32" t="n">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="G32" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Main</t>
+          <t>Instantiation</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>/docstring</t>
+          <t>/instantiation/parameter.a</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -2252,13 +2190,13 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="E33" t="n">
         <v>3</v>
       </c>
       <c r="F33" t="n">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="G33" t="n">
         <v>3</v>
@@ -2267,41 +2205,41 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Main</t>
+          <t>Instantiation</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>/docstring</t>
+          <t>/instantiation/parameter.a</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>&lt;class 'str'&gt;</t>
+          <t>&lt;class 'int'&gt;</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="E34" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F34" t="n">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="G34" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Main</t>
+          <t>Instantiation</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>/docstring</t>
+          <t>/instantiation/parameter.b</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -2310,13 +2248,13 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="E35" t="n">
         <v>3</v>
       </c>
       <c r="F35" t="n">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="G35" t="n">
         <v>3</v>
@@ -2325,41 +2263,41 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Main</t>
+          <t>Instantiation</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>/docstring</t>
+          <t>/instantiation/parameter.b</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>&lt;class 'str'&gt;</t>
+          <t>&lt;class 'int'&gt;</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="E36" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F36" t="n">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="G36" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Main</t>
+          <t>Instantiation</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>/docstring</t>
+          <t>/instantiation/parameter.c</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -2368,13 +2306,13 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="E37" t="n">
         <v>3</v>
       </c>
       <c r="F37" t="n">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="G37" t="n">
         <v>3</v>
@@ -2388,25 +2326,25 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>/instantiation</t>
+          <t>/instantiation/parameter.c</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>&lt;class 'str'&gt;</t>
+          <t>&lt;class 'int'&gt;</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E38" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F38" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G38" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39">
@@ -2417,7 +2355,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>/instantiation/parameter.a</t>
+          <t>/instantiation/parameter.d</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -2426,13 +2364,13 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E39" t="n">
         <v>3</v>
       </c>
       <c r="F39" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G39" t="n">
         <v>3</v>
@@ -2446,7 +2384,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>/instantiation/parameter.a</t>
+          <t>/instantiation/parameter.d</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -2455,13 +2393,13 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E40" t="n">
         <v>4</v>
       </c>
       <c r="F40" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G40" t="n">
         <v>4</v>
@@ -2470,12 +2408,12 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Instantiation</t>
+          <t>_step_1</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>/instantiation/parameter.b</t>
+          <t>/steps/_step_1/name</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -2484,56 +2422,56 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Instantiation</t>
+          <t>_step_1</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>/instantiation/parameter.b</t>
+          <t>/steps/_step_1/name</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>&lt;class 'int'&gt;</t>
+          <t>&lt;class 'str'&gt;</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E42" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F42" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G42" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Instantiation</t>
+          <t>_step_1</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>/instantiation/parameter.c</t>
+          <t>/steps/_step_1/method_name</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -2545,53 +2483,53 @@
         <v>4</v>
       </c>
       <c r="E43" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F43" t="n">
         <v>4</v>
       </c>
       <c r="G43" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Instantiation</t>
+          <t>_step_1</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>/instantiation/parameter.c</t>
+          <t>/steps/_step_1/method_name</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>&lt;class 'int'&gt;</t>
+          <t>&lt;class 'str'&gt;</t>
         </is>
       </c>
       <c r="D44" t="n">
         <v>4</v>
       </c>
       <c r="E44" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F44" t="n">
         <v>4</v>
       </c>
       <c r="G44" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Instantiation</t>
+          <t>_step_1</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>/instantiation/parameter.d</t>
+          <t>/steps/_step_1/docstring</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -2600,45 +2538,45 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E45" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F45" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G45" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Instantiation</t>
+          <t>_step_1</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>/instantiation/parameter.d</t>
+          <t>/steps/_step_1/docstring</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>&lt;class 'int'&gt;</t>
+          <t>&lt;class 'str'&gt;</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E46" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F46" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G46" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47">
@@ -2649,7 +2587,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>/steps/_step_1/name</t>
+          <t>/steps/_step_1/uses</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -2658,13 +2596,13 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E47" t="n">
         <v>2</v>
       </c>
       <c r="F47" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G47" t="n">
         <v>2</v>
@@ -2678,7 +2616,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>/steps/_step_1/name</t>
+          <t>/steps/_step_1/uses</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2687,13 +2625,13 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E48" t="n">
         <v>3</v>
       </c>
       <c r="F48" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G48" t="n">
         <v>3</v>
@@ -2707,7 +2645,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>/steps/_step_1/method_name</t>
+          <t>/steps/_step_1/impacts</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -2716,13 +2654,13 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E49" t="n">
         <v>2</v>
       </c>
       <c r="F49" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G49" t="n">
         <v>2</v>
@@ -2736,7 +2674,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>/steps/_step_1/method_name</t>
+          <t>/steps/_step_1/impacts</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2745,13 +2683,13 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E50" t="n">
         <v>3</v>
       </c>
       <c r="F50" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G50" t="n">
         <v>3</v>
@@ -2765,7 +2703,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>/steps/_step_1/docstring</t>
+          <t>/steps/_step_1/metadata</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2774,13 +2712,13 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E51" t="n">
         <v>2</v>
       </c>
       <c r="F51" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="G51" t="n">
         <v>2</v>
@@ -2794,7 +2732,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>/steps/_step_1/docstring</t>
+          <t>/steps/_step_1/metadata</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -2803,13 +2741,13 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E52" t="n">
         <v>3</v>
       </c>
       <c r="F52" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="G52" t="n">
         <v>3</v>
@@ -2823,7 +2761,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>/steps/_step_1/uses</t>
+          <t>/steps/_step_1/output</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2832,13 +2770,13 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E53" t="n">
         <v>2</v>
       </c>
       <c r="F53" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="G53" t="n">
         <v>2</v>
@@ -2852,7 +2790,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>/steps/_step_1/uses</t>
+          <t>/steps/_step_1/output/intermediate.ret_1</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2861,13 +2799,13 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E54" t="n">
         <v>3</v>
       </c>
       <c r="F54" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="G54" t="n">
         <v>3</v>
@@ -2881,36 +2819,36 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>/steps/_step_1/impacts</t>
+          <t>/steps/_step_1/output/intermediate.ret_1</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>&lt;class 'str'&gt;</t>
+          <t>&lt;class 'int'&gt;</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E55" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F55" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G55" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>_step_1</t>
+          <t>_step_2</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>/steps/_step_1/impacts</t>
+          <t>/steps/_step_2/name</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2919,27 +2857,27 @@
         </is>
       </c>
       <c r="D56" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E56" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F56" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G56" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>_step_1</t>
+          <t>_step_2</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>/steps/_step_1/metadata</t>
+          <t>/steps/_step_2/name</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2948,27 +2886,27 @@
         </is>
       </c>
       <c r="D57" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E57" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F57" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="G57" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>_step_1</t>
+          <t>_step_2</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>/steps/_step_1/metadata</t>
+          <t>/steps/_step_2/method_name</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2977,27 +2915,27 @@
         </is>
       </c>
       <c r="D58" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E58" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F58" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G58" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>_step_1</t>
+          <t>_step_2</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>/steps/_step_1/output</t>
+          <t>/steps/_step_2/method_name</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -3006,27 +2944,27 @@
         </is>
       </c>
       <c r="D59" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="E59" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F59" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="G59" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>_step_1</t>
+          <t>_step_2</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>/steps/_step_1/output/intermediate.ret_1</t>
+          <t>/steps/_step_2/docstring</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -3035,45 +2973,45 @@
         </is>
       </c>
       <c r="D60" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E60" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F60" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G60" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>_step_1</t>
+          <t>_step_2</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>/steps/_step_1/output/intermediate.ret_1</t>
+          <t>/steps/_step_2/docstring</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>&lt;class 'int'&gt;</t>
+          <t>&lt;class 'str'&gt;</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E61" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F61" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G61" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="62">
@@ -3084,7 +3022,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>/steps/_step_2/name</t>
+          <t>/steps/_step_2/uses</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -3093,13 +3031,13 @@
         </is>
       </c>
       <c r="D62" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E62" t="n">
         <v>2</v>
       </c>
       <c r="F62" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G62" t="n">
         <v>2</v>
@@ -3113,7 +3051,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>/steps/_step_2/name</t>
+          <t>/steps/_step_2/uses</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -3122,13 +3060,13 @@
         </is>
       </c>
       <c r="D63" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E63" t="n">
         <v>3</v>
       </c>
       <c r="F63" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G63" t="n">
         <v>3</v>
@@ -3142,7 +3080,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>/steps/_step_2/method_name</t>
+          <t>/steps/_step_2/impacts</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -3151,13 +3089,13 @@
         </is>
       </c>
       <c r="D64" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E64" t="n">
         <v>2</v>
       </c>
       <c r="F64" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G64" t="n">
         <v>2</v>
@@ -3171,7 +3109,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>/steps/_step_2/method_name</t>
+          <t>/steps/_step_2/impacts</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -3180,13 +3118,13 @@
         </is>
       </c>
       <c r="D65" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E65" t="n">
         <v>3</v>
       </c>
       <c r="F65" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G65" t="n">
         <v>3</v>
@@ -3200,7 +3138,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>/steps/_step_2/docstring</t>
+          <t>/steps/_step_2/metadata</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -3209,13 +3147,13 @@
         </is>
       </c>
       <c r="D66" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E66" t="n">
         <v>2</v>
       </c>
       <c r="F66" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="G66" t="n">
         <v>2</v>
@@ -3229,7 +3167,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>/steps/_step_2/docstring</t>
+          <t>/steps/_step_2/metadata</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -3238,13 +3176,13 @@
         </is>
       </c>
       <c r="D67" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E67" t="n">
         <v>3</v>
       </c>
       <c r="F67" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="G67" t="n">
         <v>3</v>
@@ -3258,7 +3196,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>/steps/_step_2/uses</t>
+          <t>/steps/_step_2/output</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -3267,13 +3205,13 @@
         </is>
       </c>
       <c r="D68" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E68" t="n">
         <v>2</v>
       </c>
       <c r="F68" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="G68" t="n">
         <v>2</v>
@@ -3287,7 +3225,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>/steps/_step_2/uses</t>
+          <t>/steps/_step_2/output/intermediate.ret_2</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -3296,13 +3234,13 @@
         </is>
       </c>
       <c r="D69" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E69" t="n">
         <v>3</v>
       </c>
       <c r="F69" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="G69" t="n">
         <v>3</v>
@@ -3316,36 +3254,36 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>/steps/_step_2/impacts</t>
+          <t>/steps/_step_2/output/intermediate.ret_2</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>&lt;class 'str'&gt;</t>
+          <t>&lt;class 'int'&gt;</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E70" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F70" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G70" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>_step_2</t>
+          <t>_step_3</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>/steps/_step_2/impacts</t>
+          <t>/steps/_step_3/name</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -3354,27 +3292,27 @@
         </is>
       </c>
       <c r="D71" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E71" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F71" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G71" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>_step_2</t>
+          <t>_step_3</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>/steps/_step_2/metadata</t>
+          <t>/steps/_step_3/name</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -3383,27 +3321,27 @@
         </is>
       </c>
       <c r="D72" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E72" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F72" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="G72" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>_step_2</t>
+          <t>_step_3</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>/steps/_step_2/metadata</t>
+          <t>/steps/_step_3/method_name</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -3412,27 +3350,27 @@
         </is>
       </c>
       <c r="D73" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E73" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F73" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G73" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>_step_2</t>
+          <t>_step_3</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>/steps/_step_2/output</t>
+          <t>/steps/_step_3/method_name</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -3441,27 +3379,27 @@
         </is>
       </c>
       <c r="D74" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="E74" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F74" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="G74" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>_step_2</t>
+          <t>_step_3</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>/steps/_step_2/output/intermediate.ret_2</t>
+          <t>/steps/_step_3/docstring</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -3470,45 +3408,45 @@
         </is>
       </c>
       <c r="D75" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E75" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F75" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G75" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>_step_2</t>
+          <t>_step_3</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>/steps/_step_2/output/intermediate.ret_2</t>
+          <t>/steps/_step_3/docstring</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>&lt;class 'int'&gt;</t>
+          <t>&lt;class 'str'&gt;</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E76" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F76" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G76" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="77">
@@ -3519,7 +3457,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>/steps/_step_3/name</t>
+          <t>/steps/_step_3/uses</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -3528,13 +3466,13 @@
         </is>
       </c>
       <c r="D77" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E77" t="n">
         <v>2</v>
       </c>
       <c r="F77" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G77" t="n">
         <v>2</v>
@@ -3548,7 +3486,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>/steps/_step_3/name</t>
+          <t>/steps/_step_3/uses</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -3557,13 +3495,13 @@
         </is>
       </c>
       <c r="D78" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E78" t="n">
         <v>3</v>
       </c>
       <c r="F78" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G78" t="n">
         <v>3</v>
@@ -3577,7 +3515,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>/steps/_step_3/method_name</t>
+          <t>/steps/_step_3/impacts</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -3586,13 +3524,13 @@
         </is>
       </c>
       <c r="D79" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E79" t="n">
         <v>2</v>
       </c>
       <c r="F79" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G79" t="n">
         <v>2</v>
@@ -3606,7 +3544,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>/steps/_step_3/method_name</t>
+          <t>/steps/_step_3/impacts</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -3615,13 +3553,13 @@
         </is>
       </c>
       <c r="D80" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E80" t="n">
         <v>3</v>
       </c>
       <c r="F80" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G80" t="n">
         <v>3</v>
@@ -3635,7 +3573,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>/steps/_step_3/docstring</t>
+          <t>/steps/_step_3/metadata</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -3644,13 +3582,13 @@
         </is>
       </c>
       <c r="D81" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E81" t="n">
         <v>2</v>
       </c>
       <c r="F81" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="G81" t="n">
         <v>2</v>
@@ -3664,7 +3602,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>/steps/_step_3/docstring</t>
+          <t>/steps/_step_3/metadata</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -3673,13 +3611,13 @@
         </is>
       </c>
       <c r="D82" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E82" t="n">
         <v>3</v>
       </c>
       <c r="F82" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="G82" t="n">
         <v>3</v>
@@ -3693,7 +3631,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>/steps/_step_3/uses</t>
+          <t>/steps/_step_3/output</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -3702,13 +3640,13 @@
         </is>
       </c>
       <c r="D83" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E83" t="n">
         <v>2</v>
       </c>
       <c r="F83" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="G83" t="n">
         <v>2</v>
@@ -3722,7 +3660,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>/steps/_step_3/uses</t>
+          <t>/steps/_step_3/output/return.ret_3</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -3731,13 +3669,13 @@
         </is>
       </c>
       <c r="D84" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E84" t="n">
         <v>3</v>
       </c>
       <c r="F84" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="G84" t="n">
         <v>3</v>
@@ -3751,36 +3689,36 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>/steps/_step_3/impacts</t>
+          <t>/steps/_step_3/output/return.ret_3</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>&lt;class 'str'&gt;</t>
+          <t>&lt;class 'int'&gt;</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E85" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F85" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G85" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>_step_3</t>
+          <t>Output</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>/steps/_step_3/impacts</t>
+          <t>/output</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -3789,27 +3727,27 @@
         </is>
       </c>
       <c r="D86" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E86" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F86" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G86" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>_step_3</t>
+          <t>Output</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>/steps/_step_3/metadata</t>
+          <t>/output/ret_3</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -3818,56 +3756,56 @@
         </is>
       </c>
       <c r="D87" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E87" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F87" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="G87" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>_step_3</t>
+          <t>Output</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>/steps/_step_3/metadata</t>
+          <t>/output/ret_3</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>&lt;class 'str'&gt;</t>
+          <t>&lt;class 'int'&gt;</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E88" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F88" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="G88" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>_step_3</t>
+          <t>Config</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>/steps/_step_3/output</t>
+          <t>/config</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -3876,13 +3814,13 @@
         </is>
       </c>
       <c r="D89" t="n">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="E89" t="n">
         <v>2</v>
       </c>
       <c r="F89" t="n">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="G89" t="n">
         <v>2</v>
@@ -3891,12 +3829,12 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>_step_3</t>
+          <t>Config</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>/steps/_step_3/output/return.ret_3</t>
+          <t>/config/show_signature</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -3905,13 +3843,13 @@
         </is>
       </c>
       <c r="D90" t="n">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="E90" t="n">
         <v>3</v>
       </c>
       <c r="F90" t="n">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="G90" t="n">
         <v>3</v>
@@ -3920,27 +3858,27 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>_step_3</t>
+          <t>Config</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>/steps/_step_3/output/return.ret_3</t>
+          <t>/config/show_signature</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>&lt;class 'int'&gt;</t>
+          <t>&lt;class 'str'&gt;</t>
         </is>
       </c>
       <c r="D91" t="n">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="E91" t="n">
         <v>4</v>
       </c>
       <c r="F91" t="n">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="G91" t="n">
         <v>4</v>
@@ -3949,12 +3887,12 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Output</t>
+          <t>Config</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>/output</t>
+          <t>/config/show_docstring</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -3963,27 +3901,27 @@
         </is>
       </c>
       <c r="D92" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E92" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F92" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G92" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Output</t>
+          <t>Config</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>/output/ret_3</t>
+          <t>/config/show_docstring</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -3992,45 +3930,45 @@
         </is>
       </c>
       <c r="D93" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E93" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F93" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G93" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Output</t>
+          <t>Config</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>/output/ret_3</t>
+          <t>/config/show_steps</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>&lt;class 'int'&gt;</t>
+          <t>&lt;class 'str'&gt;</t>
         </is>
       </c>
       <c r="D94" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E94" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F94" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G94" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="95">
@@ -4041,7 +3979,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>/config</t>
+          <t>/config/show_steps</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -4050,16 +3988,16 @@
         </is>
       </c>
       <c r="D95" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E95" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F95" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G95" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="96">
@@ -4070,7 +4008,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>/config/show_signature</t>
+          <t>/config/step_config</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -4079,13 +4017,13 @@
         </is>
       </c>
       <c r="D96" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E96" t="n">
         <v>3</v>
       </c>
       <c r="F96" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G96" t="n">
         <v>3</v>
@@ -4099,7 +4037,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>/config/show_signature</t>
+          <t>/config/step_config/show_method_name</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -4108,13 +4046,13 @@
         </is>
       </c>
       <c r="D97" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E97" t="n">
         <v>4</v>
       </c>
       <c r="F97" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G97" t="n">
         <v>4</v>
@@ -4128,7 +4066,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>/config/show_docstring</t>
+          <t>/config/step_config/show_method_name</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -4137,16 +4075,16 @@
         </is>
       </c>
       <c r="D98" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E98" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F98" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G98" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="99">
@@ -4157,7 +4095,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>/config/show_docstring</t>
+          <t>/config/step_config/show_docstring</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -4166,13 +4104,13 @@
         </is>
       </c>
       <c r="D99" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E99" t="n">
         <v>4</v>
       </c>
       <c r="F99" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G99" t="n">
         <v>4</v>
@@ -4186,7 +4124,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>/config/show_steps</t>
+          <t>/config/step_config/show_docstring</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -4195,16 +4133,16 @@
         </is>
       </c>
       <c r="D100" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E100" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F100" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G100" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="101">
@@ -4215,7 +4153,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>/config/show_steps</t>
+          <t>/config/step_config/show_uses</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -4224,13 +4162,13 @@
         </is>
       </c>
       <c r="D101" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E101" t="n">
         <v>4</v>
       </c>
       <c r="F101" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G101" t="n">
         <v>4</v>
@@ -4244,7 +4182,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>/config/step_config</t>
+          <t>/config/step_config/show_uses</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -4253,16 +4191,16 @@
         </is>
       </c>
       <c r="D102" t="n">
+        <v>7</v>
+      </c>
+      <c r="E102" t="n">
         <v>5</v>
       </c>
-      <c r="E102" t="n">
-        <v>3</v>
-      </c>
       <c r="F102" t="n">
+        <v>7</v>
+      </c>
+      <c r="G102" t="n">
         <v>5</v>
-      </c>
-      <c r="G102" t="n">
-        <v>3</v>
       </c>
     </row>
     <row r="103">
@@ -4273,7 +4211,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>/config/step_config/show_method_name</t>
+          <t>/config/step_config/show_impacts</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -4282,13 +4220,13 @@
         </is>
       </c>
       <c r="D103" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E103" t="n">
         <v>4</v>
       </c>
       <c r="F103" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G103" t="n">
         <v>4</v>
@@ -4302,7 +4240,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>/config/step_config/show_method_name</t>
+          <t>/config/step_config/show_impacts</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -4311,13 +4249,13 @@
         </is>
       </c>
       <c r="D104" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E104" t="n">
         <v>5</v>
       </c>
       <c r="F104" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G104" t="n">
         <v>5</v>
@@ -4331,7 +4269,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>/config/step_config/show_docstring</t>
+          <t>/config/step_config/show_output</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -4340,13 +4278,13 @@
         </is>
       </c>
       <c r="D105" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E105" t="n">
         <v>4</v>
       </c>
       <c r="F105" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G105" t="n">
         <v>4</v>
@@ -4360,7 +4298,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>/config/step_config/show_docstring</t>
+          <t>/config/step_config/show_output</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -4369,13 +4307,13 @@
         </is>
       </c>
       <c r="D106" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E106" t="n">
         <v>5</v>
       </c>
       <c r="F106" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G106" t="n">
         <v>5</v>
@@ -4389,7 +4327,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>/config/step_config/show_uses</t>
+          <t>/config/step_config/show_metadata</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -4398,13 +4336,13 @@
         </is>
       </c>
       <c r="D107" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E107" t="n">
         <v>4</v>
       </c>
       <c r="F107" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G107" t="n">
         <v>4</v>
@@ -4418,7 +4356,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>/config/step_config/show_uses</t>
+          <t>/config/step_config/show_metadata</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -4427,189 +4365,15 @@
         </is>
       </c>
       <c r="D108" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E108" t="n">
         <v>5</v>
       </c>
       <c r="F108" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G108" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="inlineStr">
-        <is>
-          <t>Config</t>
-        </is>
-      </c>
-      <c r="B109" t="inlineStr">
-        <is>
-          <t>/config/step_config/show_impacts</t>
-        </is>
-      </c>
-      <c r="C109" t="inlineStr">
-        <is>
-          <t>&lt;class 'str'&gt;</t>
-        </is>
-      </c>
-      <c r="D109" t="n">
-        <v>8</v>
-      </c>
-      <c r="E109" t="n">
-        <v>4</v>
-      </c>
-      <c r="F109" t="n">
-        <v>8</v>
-      </c>
-      <c r="G109" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" t="inlineStr">
-        <is>
-          <t>Config</t>
-        </is>
-      </c>
-      <c r="B110" t="inlineStr">
-        <is>
-          <t>/config/step_config/show_impacts</t>
-        </is>
-      </c>
-      <c r="C110" t="inlineStr">
-        <is>
-          <t>&lt;class 'str'&gt;</t>
-        </is>
-      </c>
-      <c r="D110" t="n">
-        <v>8</v>
-      </c>
-      <c r="E110" t="n">
-        <v>5</v>
-      </c>
-      <c r="F110" t="n">
-        <v>8</v>
-      </c>
-      <c r="G110" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" t="inlineStr">
-        <is>
-          <t>Config</t>
-        </is>
-      </c>
-      <c r="B111" t="inlineStr">
-        <is>
-          <t>/config/step_config/show_output</t>
-        </is>
-      </c>
-      <c r="C111" t="inlineStr">
-        <is>
-          <t>&lt;class 'str'&gt;</t>
-        </is>
-      </c>
-      <c r="D111" t="n">
-        <v>9</v>
-      </c>
-      <c r="E111" t="n">
-        <v>4</v>
-      </c>
-      <c r="F111" t="n">
-        <v>9</v>
-      </c>
-      <c r="G111" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="inlineStr">
-        <is>
-          <t>Config</t>
-        </is>
-      </c>
-      <c r="B112" t="inlineStr">
-        <is>
-          <t>/config/step_config/show_output</t>
-        </is>
-      </c>
-      <c r="C112" t="inlineStr">
-        <is>
-          <t>&lt;class 'str'&gt;</t>
-        </is>
-      </c>
-      <c r="D112" t="n">
-        <v>9</v>
-      </c>
-      <c r="E112" t="n">
-        <v>5</v>
-      </c>
-      <c r="F112" t="n">
-        <v>9</v>
-      </c>
-      <c r="G112" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" t="inlineStr">
-        <is>
-          <t>Config</t>
-        </is>
-      </c>
-      <c r="B113" t="inlineStr">
-        <is>
-          <t>/config/step_config/show_metadata</t>
-        </is>
-      </c>
-      <c r="C113" t="inlineStr">
-        <is>
-          <t>&lt;class 'str'&gt;</t>
-        </is>
-      </c>
-      <c r="D113" t="n">
-        <v>10</v>
-      </c>
-      <c r="E113" t="n">
-        <v>4</v>
-      </c>
-      <c r="F113" t="n">
-        <v>10</v>
-      </c>
-      <c r="G113" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" t="inlineStr">
-        <is>
-          <t>Config</t>
-        </is>
-      </c>
-      <c r="B114" t="inlineStr">
-        <is>
-          <t>/config/step_config/show_metadata</t>
-        </is>
-      </c>
-      <c r="C114" t="inlineStr">
-        <is>
-          <t>&lt;class 'str'&gt;</t>
-        </is>
-      </c>
-      <c r="D114" t="n">
-        <v>10</v>
-      </c>
-      <c r="E114" t="n">
-        <v>5</v>
-      </c>
-      <c r="F114" t="n">
-        <v>10</v>
-      </c>
-      <c r="G114" t="n">
         <v>5</v>
       </c>
     </row>

</xml_diff>